<commit_message>
Added changelog; updated accessories; updated bom
</commit_message>
<xml_diff>
--- a/fbcBOM.xlsx
+++ b/fbcBOM.xlsx
@@ -7,7 +7,7 @@
     <sheet state="visible" name="&lt;=V1.2" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">v1.3!$A$2:$F$56</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">v1.3!$A$2:$F$57</definedName>
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">'&lt;=V1.2'!$A$2:$F$57</definedName>
   </definedNames>
   <calcPr/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="205">
   <si>
     <t>Frog Boy Color BOM for board revision v1.3</t>
   </si>
@@ -281,7 +281,7 @@
     <t>https://www.mouser.com/ProductDetail/621-DMP6350SQ-7</t>
   </si>
   <si>
-    <t>R1,R10,R12, R17</t>
+    <t>R1,R10,R12</t>
   </si>
   <si>
     <t>10K</t>
@@ -290,322 +290,331 @@
     <t>https://www.mouser.com/ProductDetail/71-CRCW0603-5.1K-E3</t>
   </si>
   <si>
+    <t>R8, R11, R19</t>
+  </si>
+  <si>
+    <t>5.1K</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>100K</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/603-RC0603FR-07100KL</t>
+  </si>
+  <si>
+    <t>R18,R20</t>
+  </si>
+  <si>
+    <t>5.6K</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/71-CRCW0603-5.6K-E3</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/603-RC0603FR-07100RL</t>
+  </si>
+  <si>
+    <t>R21,R14</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/603-RT0603FRE13150RL</t>
+  </si>
+  <si>
+    <t>R23</t>
+  </si>
+  <si>
+    <t>430K</t>
+  </si>
+  <si>
+    <t>0605</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/603-RC0603FR-13430KL</t>
+  </si>
+  <si>
+    <t>R24</t>
+  </si>
+  <si>
+    <t>20K</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/603-RC0603FR-0720KL</t>
+  </si>
+  <si>
+    <t>R25</t>
+  </si>
+  <si>
+    <t>47K</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/603-RC0603FR-0747KL</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>1.5M</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/71-CRCW0603-1.5M-E3</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>200K</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/603-RC0603FR-07200KL</t>
+  </si>
+  <si>
+    <t>R5,R22</t>
+  </si>
+  <si>
+    <t>3.3K</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/71-CRCW0603-3.3K-E3</t>
+  </si>
+  <si>
+    <t>R6, R16</t>
+  </si>
+  <si>
+    <t>49.9K</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/71-CRCW0603-49.9K-E3</t>
+  </si>
+  <si>
+    <t>R7,R19</t>
+  </si>
+  <si>
+    <t>2.2K</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/71-CRCW0603-2.2K-E3</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>1K</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/652-CR0603FX-1001ELF</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>15K</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Bourns/CR0603-FX-1502ELF</t>
+  </si>
+  <si>
+    <t>RN1</t>
+  </si>
+  <si>
+    <t>270x4</t>
+  </si>
+  <si>
+    <t>Can harvest from GBC: RA3</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/603-TC164-JR-07270RL</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>SKRTLAE010</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/688-SKRTLA</t>
+  </si>
+  <si>
+    <t>SW8,SW7,SW5,SW3,SW1,SW2,SW4,SW6</t>
+  </si>
+  <si>
+    <t>SKRRAAE010</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/688-SKRRAA</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>CGB CPU</t>
+  </si>
+  <si>
+    <t>U10</t>
+  </si>
+  <si>
+    <t>MAX16054AZT+T</t>
+  </si>
+  <si>
+    <t>SOT-23-6</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/700-MAX16054AZTT</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>CGB RAM</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>BQ24072TRGTR</t>
+  </si>
+  <si>
+    <t>VQFN-16</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/595-BQ24072TRGTR</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>TPS61202DSC</t>
+  </si>
+  <si>
+    <t>WSON-10</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/595-TPS61202DSCR</t>
+  </si>
+  <si>
+    <t>U5,U6</t>
+  </si>
+  <si>
+    <t>LM4875MM_NOPB</t>
+  </si>
+  <si>
+    <t>VSSOP-8</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/926-LM4875MM-NOPB</t>
+  </si>
+  <si>
+    <t>U7</t>
+  </si>
+  <si>
+    <t>MCP1700T-3302E/TT</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/579-MCP1700T3302E-TT</t>
+  </si>
+  <si>
+    <t>U8</t>
+  </si>
+  <si>
+    <t>TLV803EB33VDBZR</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/595-TLV803EB33VDBZR</t>
+  </si>
+  <si>
+    <t>U9</t>
+  </si>
+  <si>
+    <t>TLV3201AIDBVR</t>
+  </si>
+  <si>
+    <t>SOT-23-5</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/595-TLV3201AIDBVR</t>
+  </si>
+  <si>
+    <t>VR1</t>
+  </si>
+  <si>
+    <t>RK08H113003Q</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/688-RK08H113003Q</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>8.388608MHz</t>
+  </si>
+  <si>
+    <t>Speaker</t>
+  </si>
+  <si>
+    <t>CMS-151103-088SP</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/490-CMS-151103-088SP</t>
+  </si>
+  <si>
+    <t>Battery</t>
+  </si>
+  <si>
+    <t>802040</t>
+  </si>
+  <si>
+    <t>Only one battery is necessary. When using two, balance charge prior to installation.</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.us/item/3256802244810488.html</t>
+  </si>
+  <si>
+    <t>Frog Boy Color BOM for board revision &lt;= v1.2</t>
+  </si>
+  <si>
+    <t>Designators</t>
+  </si>
+  <si>
+    <t>C12,C15</t>
+  </si>
+  <si>
+    <t>C7,C9,C4,C1,C5,C6,C32,C8</t>
+  </si>
+  <si>
+    <t>Optional</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/485-1769</t>
+  </si>
+  <si>
+    <t>Q3,Q2</t>
+  </si>
+  <si>
+    <t>SI2312BDS-T1-BE3</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/78-SI2312BDS-T1-BE3</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
     <t>R11,R8</t>
   </si>
   <si>
-    <t>5.1K</t>
-  </si>
-  <si>
-    <t>R15</t>
-  </si>
-  <si>
-    <t>100K</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/603-RC0603FR-07100KL</t>
-  </si>
-  <si>
-    <t>R18,R20</t>
-  </si>
-  <si>
-    <t>5.6K</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/71-CRCW0603-5.6K-E3</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/603-RC0603FR-07100RL</t>
-  </si>
-  <si>
-    <t>R21,R14</t>
-  </si>
-  <si>
-    <t>150</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/603-RT0603FRE13150RL</t>
-  </si>
-  <si>
-    <t>R23</t>
-  </si>
-  <si>
-    <t>430K</t>
-  </si>
-  <si>
-    <t>0605</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/603-RC0603FR-13430KL</t>
-  </si>
-  <si>
-    <t>R24</t>
-  </si>
-  <si>
-    <t>20K</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/603-RC0603FR-0720KL</t>
-  </si>
-  <si>
-    <t>R25</t>
-  </si>
-  <si>
-    <t>47K</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/603-RC0603FR-0747KL</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>1.5M</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/71-CRCW0603-1.5M-E3</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>200K</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/603-RC0603FR-07200KL</t>
-  </si>
-  <si>
-    <t>R5,R22</t>
-  </si>
-  <si>
-    <t>3.3K</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/71-CRCW0603-3.3K-E3</t>
-  </si>
-  <si>
-    <t>R6, R16</t>
-  </si>
-  <si>
-    <t>49.9K</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/71-CRCW0603-49.9K-E3</t>
-  </si>
-  <si>
-    <t>R7,R19</t>
-  </si>
-  <si>
-    <t>2.2K</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/71-CRCW0603-2.2K-E3</t>
-  </si>
-  <si>
-    <t>R9</t>
-  </si>
-  <si>
-    <t>1K</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/652-CR0603FX-1001ELF</t>
-  </si>
-  <si>
-    <t>RN1</t>
-  </si>
-  <si>
-    <t>270x4</t>
-  </si>
-  <si>
-    <t>Can harvest from GBC: RA3</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/603-TC164-JR-07270RL</t>
-  </si>
-  <si>
-    <t>S2</t>
-  </si>
-  <si>
-    <t>SKRTLAE010</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/688-SKRTLA</t>
-  </si>
-  <si>
-    <t>SW8,SW7,SW5,SW3,SW1,SW2,SW4,SW6</t>
-  </si>
-  <si>
-    <t>SKRRAAE010</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/688-SKRRAA</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>CGB CPU</t>
-  </si>
-  <si>
-    <t>U10</t>
-  </si>
-  <si>
-    <t>MAX16054AZT+T</t>
-  </si>
-  <si>
-    <t>SOT-23-6</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/700-MAX16054AZTT</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>CGB RAM</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>BQ24072TRGTR</t>
-  </si>
-  <si>
-    <t>VQFN-16</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/595-BQ24072TRGTR</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>TPS61202DSC</t>
-  </si>
-  <si>
-    <t>WSON-10</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/595-TPS61202DSCR</t>
-  </si>
-  <si>
-    <t>U5,U6</t>
-  </si>
-  <si>
-    <t>LM4875MM_NOPB</t>
-  </si>
-  <si>
-    <t>VSSOP-8</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/926-LM4875MM-NOPB</t>
-  </si>
-  <si>
-    <t>U7</t>
-  </si>
-  <si>
-    <t>MCP1700T-3302E/TT</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/579-MCP1700T3302E-TT</t>
-  </si>
-  <si>
-    <t>U8</t>
-  </si>
-  <si>
-    <t>TLV803EB33VDBZR</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/595-TLV803EB33VDBZR</t>
-  </si>
-  <si>
-    <t>U9</t>
-  </si>
-  <si>
-    <t>TLV3201AIDBVR</t>
-  </si>
-  <si>
-    <t>SOT-23-5</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/595-TLV3201AIDBVR</t>
-  </si>
-  <si>
-    <t>VR1</t>
-  </si>
-  <si>
-    <t>RK08H113003Q</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/688-RK08H113003Q</t>
-  </si>
-  <si>
-    <t>Y1</t>
-  </si>
-  <si>
-    <t>8.388608MHz</t>
-  </si>
-  <si>
-    <t>Speaker</t>
-  </si>
-  <si>
-    <t>CMS-151103-088SP</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/490-CMS-151103-088SP</t>
-  </si>
-  <si>
-    <t>Battery</t>
-  </si>
-  <si>
-    <t>802040</t>
-  </si>
-  <si>
-    <t>Only one battery is necessary. When using two, balance charge prior to installation.</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.us/item/3256802244810488.html</t>
-  </si>
-  <si>
-    <t>Frog Boy Color BOM for board revision &lt;= v1.2</t>
-  </si>
-  <si>
-    <t>Designators</t>
-  </si>
-  <si>
-    <t>C12,C15</t>
-  </si>
-  <si>
-    <t>C7,C9,C4,C1,C5,C6,C32,C8</t>
-  </si>
-  <si>
-    <t>Optional</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/485-1769</t>
-  </si>
-  <si>
-    <t>Q3,Q2</t>
-  </si>
-  <si>
-    <t>SI2312BDS-T1-BE3</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/78-SI2312BDS-T1-BE3</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
     <t>R13,R12,R10,R15</t>
-  </si>
-  <si>
-    <t>R17</t>
   </si>
   <si>
     <t>10k</t>
@@ -630,7 +639,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m-d"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -654,6 +663,11 @@
     <font>
       <u/>
       <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
@@ -713,7 +727,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -763,16 +777,22 @@
     <xf borderId="2" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -784,10 +804,10 @@
     <xf borderId="1" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -1471,7 +1491,7 @@
         <v>88</v>
       </c>
       <c r="B26" s="3">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>89</v>
@@ -1489,7 +1509,7 @@
         <v>91</v>
       </c>
       <c r="B27" s="3">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>92</v>
@@ -1743,33 +1763,33 @@
       <c r="B41" s="3">
         <v>1.0</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="D41" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E41" s="6" t="s">
+      <c r="D41" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="6"/>
+      <c r="F41" s="18" t="s">
         <v>135</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B42" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="B42" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="C42" s="4" t="s">
+      <c r="D42" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="D42" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E42" s="6"/>
       <c r="F42" s="7" t="s">
         <v>139</v>
       </c>
@@ -1779,7 +1799,7 @@
         <v>140</v>
       </c>
       <c r="B43" s="3">
-        <v>8.0</v>
+        <v>1.0</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>141</v>
@@ -1797,7 +1817,7 @@
         <v>143</v>
       </c>
       <c r="B44" s="3">
-        <v>1.0</v>
+        <v>8.0</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>144</v>
@@ -1805,112 +1825,113 @@
       <c r="D44" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E44" s="6" t="s">
-        <v>64</v>
+      <c r="E44" s="6"/>
+      <c r="F44" s="7" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B45" s="3">
         <v>1.0</v>
       </c>
-      <c r="C45" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="D45" s="3" t="s">
+      <c r="C45" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="F45" s="8" t="s">
-        <v>148</v>
+      <c r="D45" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B46" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C46" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="B46" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="C46" s="4" t="s">
+      <c r="D46" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="D46" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>64</v>
+      <c r="F46" s="8" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B47" s="3">
         <v>1.0</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="D47" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="E47" s="6"/>
-      <c r="F47" s="7" t="s">
-        <v>154</v>
+      <c r="D47" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B48" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C48" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="B48" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="C48" s="4" t="s">
+      <c r="D48" s="19" t="s">
         <v>156</v>
-      </c>
-      <c r="D48" s="18" t="s">
-        <v>157</v>
       </c>
       <c r="E48" s="6"/>
       <c r="F48" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B49" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C49" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="B49" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="C49" s="4" t="s">
+      <c r="D49" s="20" t="s">
         <v>160</v>
-      </c>
-      <c r="D49" s="17" t="s">
-        <v>161</v>
       </c>
       <c r="E49" s="6"/>
       <c r="F49" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B50" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="C50" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="B50" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="C50" s="3" t="s">
+      <c r="D50" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="D50" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F50" s="8" t="s">
+      <c r="E50" s="6"/>
+      <c r="F50" s="7" t="s">
         <v>165</v>
       </c>
     </row>
@@ -1921,14 +1942,13 @@
       <c r="B51" s="3">
         <v>1.0</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="D51" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="6"/>
-      <c r="F51" s="7" t="s">
+      <c r="F51" s="8" t="s">
         <v>168</v>
       </c>
     </row>
@@ -1943,22 +1963,22 @@
         <v>170</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>171</v>
+        <v>86</v>
       </c>
       <c r="E52" s="6"/>
       <c r="F52" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B53" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C53" s="4" t="s">
         <v>173</v>
-      </c>
-      <c r="B53" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>174</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>174</v>
@@ -1979,67 +1999,46 @@
         <v>177</v>
       </c>
       <c r="D54" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="E54" s="6"/>
+      <c r="F54" s="7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B55" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D55" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E54" s="6" t="s">
+      <c r="E55" s="6" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="B55" s="19">
-        <v>2.0</v>
-      </c>
-      <c r="C55" s="20" t="s">
-        <v>179</v>
-      </c>
-      <c r="D55" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E55" s="6"/>
-      <c r="F55" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="G55" s="6"/>
-      <c r="H55" s="6"/>
-      <c r="I55" s="6"/>
-      <c r="J55" s="6"/>
-      <c r="K55" s="6"/>
-      <c r="L55" s="6"/>
-      <c r="M55" s="6"/>
-      <c r="N55" s="6"/>
-      <c r="O55" s="6"/>
-      <c r="P55" s="6"/>
-      <c r="Q55" s="6"/>
-      <c r="R55" s="6"/>
-      <c r="S55" s="6"/>
-      <c r="T55" s="6"/>
-      <c r="U55" s="6"/>
-      <c r="V55" s="6"/>
-      <c r="W55" s="6"/>
-      <c r="X55" s="6"/>
-      <c r="Y55" s="6"/>
     </row>
     <row r="56">
       <c r="A56" s="6" t="s">
         <v>181</v>
       </c>
       <c r="B56" s="21">
-        <v>44928.0</v>
-      </c>
-      <c r="C56" s="6" t="s">
+        <v>2.0</v>
+      </c>
+      <c r="C56" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="D56" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D56" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="E56" s="6" t="s">
+      <c r="E56" s="6"/>
+      <c r="F56" s="7" t="s">
         <v>183</v>
-      </c>
-      <c r="F56" s="7" t="s">
-        <v>184</v>
       </c>
       <c r="G56" s="6"/>
       <c r="H56" s="6"/>
@@ -2061,10 +2060,49 @@
       <c r="X56" s="6"/>
       <c r="Y56" s="6"/>
     </row>
+    <row r="57">
+      <c r="A57" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="B57" s="23">
+        <v>44928.0</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="G57" s="6"/>
+      <c r="H57" s="6"/>
+      <c r="I57" s="6"/>
+      <c r="J57" s="6"/>
+      <c r="K57" s="6"/>
+      <c r="L57" s="6"/>
+      <c r="M57" s="6"/>
+      <c r="N57" s="6"/>
+      <c r="O57" s="6"/>
+      <c r="P57" s="6"/>
+      <c r="Q57" s="6"/>
+      <c r="R57" s="6"/>
+      <c r="S57" s="6"/>
+      <c r="T57" s="6"/>
+      <c r="U57" s="6"/>
+      <c r="V57" s="6"/>
+      <c r="W57" s="6"/>
+      <c r="X57" s="6"/>
+      <c r="Y57" s="6"/>
+    </row>
   </sheetData>
-  <autoFilter ref="$A$2:$F$56">
-    <sortState ref="A2:F56">
-      <sortCondition ref="A2:A56"/>
+  <autoFilter ref="$A$2:$F$57">
+    <sortState ref="A2:F57">
+      <sortCondition ref="A2:A57"/>
     </sortState>
   </autoFilter>
   <mergeCells count="1">
@@ -2108,18 +2146,19 @@
     <hyperlink r:id="rId35" ref="F41"/>
     <hyperlink r:id="rId36" ref="F42"/>
     <hyperlink r:id="rId37" ref="F43"/>
-    <hyperlink r:id="rId38" ref="F45"/>
-    <hyperlink r:id="rId39" ref="F47"/>
+    <hyperlink r:id="rId38" ref="F44"/>
+    <hyperlink r:id="rId39" ref="F46"/>
     <hyperlink r:id="rId40" ref="F48"/>
     <hyperlink r:id="rId41" ref="F49"/>
     <hyperlink r:id="rId42" ref="F50"/>
     <hyperlink r:id="rId43" ref="F51"/>
     <hyperlink r:id="rId44" ref="F52"/>
     <hyperlink r:id="rId45" ref="F53"/>
-    <hyperlink r:id="rId46" ref="F55"/>
+    <hyperlink r:id="rId46" ref="F54"/>
     <hyperlink r:id="rId47" ref="F56"/>
+    <hyperlink r:id="rId48" ref="F57"/>
   </hyperlinks>
-  <drawing r:id="rId48"/>
+  <drawing r:id="rId49"/>
 </worksheet>
 </file>
 
@@ -2142,7 +2181,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>0</v>
@@ -2156,7 +2195,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -2184,7 +2223,7 @@
       <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="24" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -2193,7 +2232,7 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B4" s="3">
         <v>2.0</v>
@@ -2201,7 +2240,7 @@
       <c r="C4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="24" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -2221,7 +2260,7 @@
       <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="24" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="8" t="s">
@@ -2238,7 +2277,7 @@
       <c r="C6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="24" t="s">
         <v>9</v>
       </c>
       <c r="F6" s="8" t="s">
@@ -2255,7 +2294,7 @@
       <c r="C7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="24" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -2275,7 +2314,7 @@
       <c r="C8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="24" t="s">
         <v>9</v>
       </c>
       <c r="F8" s="8" t="s">
@@ -2292,7 +2331,7 @@
       <c r="C9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="24" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="8" t="s">
@@ -2309,7 +2348,7 @@
       <c r="C10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="24" t="s">
         <v>9</v>
       </c>
       <c r="F10" s="8" t="s">
@@ -2326,7 +2365,7 @@
       <c r="C11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="24" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="8" t="s">
@@ -2343,7 +2382,7 @@
       <c r="C12" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="24" t="s">
         <v>9</v>
       </c>
       <c r="F12" s="8" t="s">
@@ -2352,7 +2391,7 @@
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B13" s="3">
         <v>8.0</v>
@@ -2360,7 +2399,7 @@
       <c r="C13" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="24" t="s">
         <v>9</v>
       </c>
       <c r="F13" s="8" t="s">
@@ -2377,7 +2416,7 @@
       <c r="C14" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="24" t="s">
         <v>9</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -2394,7 +2433,7 @@
       <c r="C15" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="24" t="s">
         <v>17</v>
       </c>
       <c r="F15" s="8" t="s">
@@ -2411,7 +2450,7 @@
       <c r="C16" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="24" t="s">
         <v>9</v>
       </c>
       <c r="F16" s="8" t="s">
@@ -2428,7 +2467,7 @@
       <c r="C17" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D17" s="24" t="s">
         <v>17</v>
       </c>
       <c r="E17" s="3" t="s">
@@ -2506,10 +2545,10 @@
         <v>60</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="22">
@@ -2582,24 +2621,24 @@
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B26" s="3">
         <v>2.0</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>86</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B27" s="3">
         <v>1.0</v>
@@ -2607,7 +2646,7 @@
       <c r="C27" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D27" s="22" t="s">
+      <c r="D27" s="24" t="s">
         <v>9</v>
       </c>
       <c r="F27" s="8" t="s">
@@ -2616,7 +2655,7 @@
     </row>
     <row r="28">
       <c r="A28" s="3" t="s">
-        <v>91</v>
+        <v>198</v>
       </c>
       <c r="B28" s="3">
         <v>2.0</v>
@@ -2624,7 +2663,7 @@
       <c r="C28" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D28" s="23" t="s">
+      <c r="D28" s="25" t="s">
         <v>9</v>
       </c>
       <c r="F28" s="8" t="s">
@@ -2633,7 +2672,7 @@
     </row>
     <row r="29">
       <c r="A29" s="3" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B29" s="3">
         <v>4.0</v>
@@ -2641,7 +2680,7 @@
       <c r="C29" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D29" s="22" t="s">
+      <c r="D29" s="24" t="s">
         <v>9</v>
       </c>
       <c r="F29" s="8" t="s">
@@ -2650,19 +2689,19 @@
     </row>
     <row r="30">
       <c r="A30" s="3" t="s">
-        <v>196</v>
+        <v>133</v>
       </c>
       <c r="B30" s="3">
         <v>1.0</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="D30" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="D30" s="24" t="s">
         <v>9</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
     <row r="31">
@@ -2675,7 +2714,7 @@
       <c r="C31" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D31" s="22" t="s">
+      <c r="D31" s="24" t="s">
         <v>9</v>
       </c>
       <c r="F31" s="8" t="s">
@@ -2689,10 +2728,10 @@
       <c r="B32" s="3">
         <v>1.0</v>
       </c>
-      <c r="C32" s="22" t="s">
+      <c r="C32" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="D32" s="22" t="s">
+      <c r="D32" s="24" t="s">
         <v>9</v>
       </c>
       <c r="F32" s="8" t="s">
@@ -2706,10 +2745,10 @@
       <c r="B33" s="3">
         <v>2.0</v>
       </c>
-      <c r="C33" s="22" t="s">
+      <c r="C33" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="D33" s="22" t="s">
+      <c r="D33" s="24" t="s">
         <v>9</v>
       </c>
       <c r="F33" s="8" t="s">
@@ -2726,7 +2765,7 @@
       <c r="C34" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D34" s="22" t="s">
+      <c r="D34" s="24" t="s">
         <v>107</v>
       </c>
       <c r="F34" s="8" t="s">
@@ -2743,7 +2782,7 @@
       <c r="C35" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D35" s="22" t="s">
+      <c r="D35" s="24" t="s">
         <v>9</v>
       </c>
       <c r="F35" s="8" t="s">
@@ -2760,7 +2799,7 @@
       <c r="C36" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="D36" s="22" t="s">
+      <c r="D36" s="24" t="s">
         <v>9</v>
       </c>
       <c r="F36" s="8" t="s">
@@ -2777,7 +2816,7 @@
       <c r="C37" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D37" s="22" t="s">
+      <c r="D37" s="24" t="s">
         <v>9</v>
       </c>
       <c r="F37" s="8" t="s">
@@ -2794,7 +2833,7 @@
       <c r="C38" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D38" s="22" t="s">
+      <c r="D38" s="24" t="s">
         <v>9</v>
       </c>
       <c r="F38" s="8" t="s">
@@ -2811,7 +2850,7 @@
       <c r="C39" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="D39" s="22" t="s">
+      <c r="D39" s="24" t="s">
         <v>9</v>
       </c>
       <c r="F39" s="8" t="s">
@@ -2828,7 +2867,7 @@
       <c r="C40" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D40" s="22" t="s">
+      <c r="D40" s="24" t="s">
         <v>9</v>
       </c>
       <c r="F40" s="8" t="s">
@@ -2837,7 +2876,7 @@
     </row>
     <row r="41">
       <c r="A41" s="3" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B41" s="3">
         <v>2.0</v>
@@ -2845,7 +2884,7 @@
       <c r="C41" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D41" s="22" t="s">
+      <c r="D41" s="24" t="s">
         <v>9</v>
       </c>
       <c r="F41" s="8" t="s">
@@ -2862,7 +2901,7 @@
       <c r="C42" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D42" s="22" t="s">
+      <c r="D42" s="24" t="s">
         <v>9</v>
       </c>
       <c r="F42" s="8" t="s">
@@ -2871,67 +2910,67 @@
     </row>
     <row r="43">
       <c r="A43" s="3" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B43" s="3">
         <v>1.0</v>
       </c>
-      <c r="C43" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="D43" s="22" t="s">
+      <c r="C43" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="D43" s="24" t="s">
         <v>17</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="3" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B44" s="3">
         <v>1.0</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>60</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B45" s="3">
         <v>8.0</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>60</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="3" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B46" s="3">
         <v>1.0</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>60</v>
@@ -2942,13 +2981,13 @@
     </row>
     <row r="47">
       <c r="A47" s="3" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B47" s="3">
         <v>1.0</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>60</v>
@@ -2959,132 +2998,132 @@
     </row>
     <row r="48">
       <c r="A48" s="3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B48" s="3">
         <v>1.0</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="D48" s="24" t="s">
-        <v>153</v>
+        <v>155</v>
+      </c>
+      <c r="D48" s="26" t="s">
+        <v>156</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="3" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B49" s="3">
         <v>1.0</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="D49" s="25" t="s">
-        <v>157</v>
+        <v>159</v>
+      </c>
+      <c r="D49" s="27" t="s">
+        <v>160</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="3" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B50" s="3">
         <v>2.0</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="D50" s="24" t="s">
-        <v>161</v>
+        <v>163</v>
+      </c>
+      <c r="D50" s="26" t="s">
+        <v>164</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="3" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B51" s="3">
         <v>1.0</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>86</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="3" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B52" s="3">
         <v>1.0</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>86</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="3" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B53" s="3">
         <v>1.0</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="3" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B54" s="3">
         <v>1.0</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="3" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B55" s="3">
         <v>1.0</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>60</v>
@@ -3095,39 +3134,39 @@
     </row>
     <row r="56">
       <c r="A56" s="3" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B56" s="3">
         <v>2.0</v>
       </c>
-      <c r="C56" s="24" t="s">
-        <v>179</v>
+      <c r="C56" s="26" t="s">
+        <v>182</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>60</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="B57" s="26">
+        <v>184</v>
+      </c>
+      <c r="B57" s="28">
         <v>44928.0</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D57" s="22" t="s">
-        <v>182</v>
+      <c r="D57" s="24" t="s">
+        <v>185</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed R19 on BOM
</commit_message>
<xml_diff>
--- a/fbcBOM.xlsx
+++ b/fbcBOM.xlsx
@@ -398,7 +398,7 @@
     <t>https://www.mouser.com/ProductDetail/71-CRCW0603-49.9K-E3</t>
   </si>
   <si>
-    <t>R7,R19</t>
+    <t>R7</t>
   </si>
   <si>
     <t>2.2K</t>
@@ -1725,7 +1725,7 @@
         <v>127</v>
       </c>
       <c r="B39" s="3">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>128</v>

</xml_diff>